<commit_message>
Added solutions and updated Daily Tracker
</commit_message>
<xml_diff>
--- a/Daily_Tracker/FINAL450.xlsx
+++ b/Daily_Tracker/FINAL450.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\myStudies\myCodingGround\Github_Official_Projects\The_Learning_Path_Github\Learn_DataStructure\Daily_Tracker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\myStudies\myCodingGround\Github_Official_Projects\LearnDataStructure\Daily_Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Question_With_URL" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2257" uniqueCount="472">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1428,6 +1429,24 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/kth-smallest-element5635/1</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/maximum-and-minimum-in-an-array/</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/write-a-program-to-reverse-an-array-or-string/</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/sort-an-array-of-0s-1s-and-2s4231/1</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/move-negative-numbers-beginning-positive-end-constant-extra-space/</t>
   </si>
 </sst>
 </file>
@@ -1869,7 +1888,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1929,8 +1948,8 @@
       <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>4</v>
+      <c r="C8" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="21">
@@ -1940,8 +1959,8 @@
       <c r="B9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>4</v>
+      <c r="C9" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="21">
@@ -1951,8 +1970,8 @@
       <c r="B10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>4</v>
+      <c r="C10" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="21">
@@ -7385,4 +7404,4175 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C481"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="28.5" customWidth="1"/>
+    <col min="2" max="2" width="123" customWidth="1"/>
+    <col min="3" max="3" width="62.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="26.25">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="B2" s="10" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="21">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="21">
+      <c r="A6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="21">
+      <c r="A7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="21">
+      <c r="A8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="21">
+      <c r="A9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="21">
+      <c r="A10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="21">
+      <c r="A11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="21">
+      <c r="A12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="21">
+      <c r="A13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="21">
+      <c r="A14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="21">
+      <c r="A15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="21">
+      <c r="A16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="21">
+      <c r="A17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="21">
+      <c r="A18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="21">
+      <c r="A19" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="21">
+      <c r="A20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="21">
+      <c r="A21" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="21">
+      <c r="A22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="21">
+      <c r="A23" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="21">
+      <c r="A24" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="21">
+      <c r="A25" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="21">
+      <c r="A26" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="21">
+      <c r="A27" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="21">
+      <c r="A28" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="21">
+      <c r="A29" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="21">
+      <c r="A30" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="21">
+      <c r="A31" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="21">
+      <c r="A32" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="21">
+      <c r="A33" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="21">
+      <c r="A34" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="21">
+      <c r="A35" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="21">
+      <c r="A36" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="21">
+      <c r="A37" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="21">
+      <c r="A38" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="21">
+      <c r="A39" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="21">
+      <c r="A40" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="21">
+      <c r="A41" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="21">
+      <c r="B42" s="7"/>
+    </row>
+    <row r="43" spans="1:2" ht="21">
+      <c r="A43" s="5"/>
+      <c r="B43" s="7"/>
+    </row>
+    <row r="44" spans="1:2" ht="21">
+      <c r="A44" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="21">
+      <c r="A45" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="21">
+      <c r="A46" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="21">
+      <c r="A47" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="21">
+      <c r="A48" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="21">
+      <c r="A49" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="21">
+      <c r="A50" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="21">
+      <c r="A51" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="21">
+      <c r="A52" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="21">
+      <c r="A53" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="21">
+      <c r="A55" s="5"/>
+      <c r="B55" s="7"/>
+    </row>
+    <row r="56" spans="1:2" ht="21">
+      <c r="A56" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="21">
+      <c r="A57" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="21">
+      <c r="A58" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="21">
+      <c r="A59" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="21">
+      <c r="A60" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="21">
+      <c r="A61" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="21">
+      <c r="A62" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="21">
+      <c r="A63" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="21">
+      <c r="A64" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="21">
+      <c r="A65" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="21">
+      <c r="A66" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="21">
+      <c r="A67" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="21">
+      <c r="A68" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="21">
+      <c r="A69" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="21">
+      <c r="A70" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="21">
+      <c r="A71" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="21">
+      <c r="A72" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="21">
+      <c r="A73" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="21">
+      <c r="A74" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="21">
+      <c r="A75" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="21">
+      <c r="A76" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="21">
+      <c r="A77" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="21">
+      <c r="A78" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="21">
+      <c r="A79" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="21">
+      <c r="A80" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="21">
+      <c r="A81" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="21">
+      <c r="A82" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="21">
+      <c r="A83" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="21">
+      <c r="A84" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="21">
+      <c r="A85" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="21">
+      <c r="A86" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="21">
+      <c r="A87" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="21">
+      <c r="A88" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="21">
+      <c r="A89" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="21">
+      <c r="A90" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="21">
+      <c r="A91" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="21">
+      <c r="A92" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="21">
+      <c r="A93" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="21">
+      <c r="A94" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B94" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="21">
+      <c r="A95" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B95" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="21">
+      <c r="A96" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B96" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="21">
+      <c r="A97" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B97" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="21">
+      <c r="A98" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B98" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="21">
+      <c r="A100" s="8"/>
+      <c r="B100" s="7"/>
+    </row>
+    <row r="101" spans="1:2" ht="21">
+      <c r="A101" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B101" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="21">
+      <c r="A102" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B102" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="21">
+      <c r="A103" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B103" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="21">
+      <c r="A104" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B104" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="21">
+      <c r="A105" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B105" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="21">
+      <c r="A106" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B106" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="21">
+      <c r="A107" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B107" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="21">
+      <c r="A108" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B108" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="21">
+      <c r="A109" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B109" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="21">
+      <c r="A110" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B110" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="21">
+      <c r="A111" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B111" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="21">
+      <c r="A112" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B112" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="21">
+      <c r="A113" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B113" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="21">
+      <c r="A114" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B114" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="21">
+      <c r="A115" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B115" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="21">
+      <c r="A116" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B116" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="21">
+      <c r="A117" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B117" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="21">
+      <c r="A118" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B118" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="21">
+      <c r="A119" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B119" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="21">
+      <c r="A120" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B120" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="21">
+      <c r="A121" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B121" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="21">
+      <c r="A122" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B122" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="21">
+      <c r="A123" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B123" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="21">
+      <c r="A124" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B124" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="21">
+      <c r="A125" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B125" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="21">
+      <c r="A126" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B126" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="21">
+      <c r="A127" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B127" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="21">
+      <c r="A128" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B128" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="21">
+      <c r="A129" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B129" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="21">
+      <c r="A130" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B130" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="21">
+      <c r="A131" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B131" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="21">
+      <c r="A132" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B132" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="21">
+      <c r="A133" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B133" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="21">
+      <c r="A134" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B134" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="21">
+      <c r="A135" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B135" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="21">
+      <c r="A136" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B136" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" ht="21">
+      <c r="B138" s="7"/>
+    </row>
+    <row r="139" spans="1:2" ht="21">
+      <c r="A139" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B139" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="21">
+      <c r="A140" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B140" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" ht="21">
+      <c r="A141" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B141" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" ht="21">
+      <c r="A142" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B142" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="21">
+      <c r="A143" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B143" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" ht="21">
+      <c r="A144" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B144" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="21">
+      <c r="A145" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B145" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="21">
+      <c r="A146" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B146" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" ht="21">
+      <c r="A147" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B147" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="21">
+      <c r="A148" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B148" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" ht="21">
+      <c r="A149" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B149" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="21">
+      <c r="A150" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B150" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" ht="21">
+      <c r="A151" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B151" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" ht="21">
+      <c r="A152" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B152" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" ht="21">
+      <c r="A153" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B153" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" ht="21">
+      <c r="A154" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B154" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" ht="21">
+      <c r="A155" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B155" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" ht="21">
+      <c r="A156" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B156" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" ht="21">
+      <c r="A157" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B157" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" ht="21">
+      <c r="A158" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B158" s="6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" ht="21">
+      <c r="A159" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B159" s="6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" ht="21">
+      <c r="A160" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B160" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" ht="21">
+      <c r="A161" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B161" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" ht="21">
+      <c r="A162" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B162" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" ht="21">
+      <c r="A163" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B163" s="6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" ht="21">
+      <c r="A164" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B164" s="7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" ht="21">
+      <c r="A165" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B165" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" ht="21">
+      <c r="A166" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B166" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" ht="21">
+      <c r="A167" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B167" s="6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" ht="21">
+      <c r="A168" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B168" s="6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" ht="21">
+      <c r="A169" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B169" s="6" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" ht="21">
+      <c r="A170" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B170" s="6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" ht="21">
+      <c r="A171" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B171" s="6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" ht="21">
+      <c r="A172" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B172" s="6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" ht="21">
+      <c r="A173" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B173" s="6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" ht="21">
+      <c r="A174" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B174" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" ht="21">
+      <c r="B176" s="7"/>
+    </row>
+    <row r="177" spans="1:2" ht="21">
+      <c r="A177" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B177" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" ht="21">
+      <c r="A178" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B178" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" ht="21">
+      <c r="A179" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B179" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" ht="21">
+      <c r="A180" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B180" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" ht="21">
+      <c r="A181" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B181" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" ht="21">
+      <c r="A182" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B182" s="6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" ht="21">
+      <c r="A183" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B183" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" ht="21">
+      <c r="A184" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B184" s="6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" ht="21">
+      <c r="A185" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B185" s="6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" ht="21">
+      <c r="A186" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B186" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" ht="21">
+      <c r="A187" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B187" s="6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" ht="21">
+      <c r="A188" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B188" s="6" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" ht="21">
+      <c r="A189" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B189" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" ht="21">
+      <c r="A190" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B190" s="6" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" ht="21">
+      <c r="A191" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B191" s="6" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" ht="21">
+      <c r="A192" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B192" s="6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" ht="21">
+      <c r="A193" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B193" s="6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" ht="21">
+      <c r="A194" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B194" s="6" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" ht="21">
+      <c r="A195" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B195" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" ht="21">
+      <c r="A196" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B196" s="6" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" ht="21">
+      <c r="A197" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B197" s="6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" ht="21">
+      <c r="A198" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B198" s="6" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" ht="21">
+      <c r="A199" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B199" s="6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" ht="21">
+      <c r="A200" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B200" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" ht="21">
+      <c r="A201" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B201" s="6" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" ht="21">
+      <c r="A202" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B202" s="6" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" ht="21">
+      <c r="A203" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B203" s="6" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" ht="21">
+      <c r="A204" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B204" s="6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" ht="21">
+      <c r="A205" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B205" s="6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" ht="21">
+      <c r="A206" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B206" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" ht="21">
+      <c r="A207" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B207" s="6" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" ht="21">
+      <c r="A208" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B208" s="6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" ht="21">
+      <c r="A209" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B209" s="6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" ht="21">
+      <c r="A210" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B210" s="6" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" ht="21">
+      <c r="A211" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B211" s="6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" ht="21">
+      <c r="A212" s="8"/>
+      <c r="B212" s="7"/>
+    </row>
+    <row r="213" spans="1:2" ht="21">
+      <c r="A213" s="8"/>
+      <c r="B213" s="7"/>
+    </row>
+    <row r="214" spans="1:2" ht="21">
+      <c r="A214" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B214" s="6" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" ht="21">
+      <c r="A215" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B215" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" ht="21">
+      <c r="A216" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B216" s="6" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" ht="21">
+      <c r="A217" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B217" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" ht="21">
+      <c r="A218" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B218" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" ht="21">
+      <c r="A219" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B219" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" ht="21">
+      <c r="A220" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B220" s="9" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" ht="21">
+      <c r="A221" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B221" s="6" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" ht="21">
+      <c r="A222" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B222" s="6" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" ht="21">
+      <c r="A223" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B223" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" ht="21">
+      <c r="A224" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B224" s="6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" ht="21">
+      <c r="A225" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B225" s="6" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" ht="21">
+      <c r="A226" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B226" s="6" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" ht="21">
+      <c r="A227" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B227" s="6" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" ht="21">
+      <c r="A228" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B228" s="6" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" ht="21">
+      <c r="A229" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B229" s="6" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" ht="21">
+      <c r="A230" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B230" s="6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" ht="21">
+      <c r="A231" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B231" s="6" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" ht="21">
+      <c r="A232" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B232" s="6" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" ht="21">
+      <c r="A233" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B233" s="6" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" ht="21">
+      <c r="A234" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B234" s="6" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" ht="21">
+      <c r="A235" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B235" s="6" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" ht="21">
+      <c r="B236" s="7"/>
+    </row>
+    <row r="237" spans="1:2" ht="21">
+      <c r="B237" s="7"/>
+    </row>
+    <row r="238" spans="1:2" ht="21">
+      <c r="A238" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B238" s="6" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" ht="21">
+      <c r="A239" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B239" s="6" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" ht="21">
+      <c r="A240" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B240" s="6" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" ht="21">
+      <c r="A241" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B241" s="6" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" ht="21">
+      <c r="A242" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B242" s="6" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" ht="21">
+      <c r="A243" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B243" s="6" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" ht="21">
+      <c r="A244" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B244" s="6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" ht="21">
+      <c r="A245" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B245" s="6" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" ht="21">
+      <c r="A246" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B246" s="6" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" ht="21">
+      <c r="A247" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B247" s="6" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" ht="21">
+      <c r="A248" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B248" s="6" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" ht="21">
+      <c r="A249" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B249" s="6" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" ht="21">
+      <c r="A250" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B250" s="6" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" ht="21">
+      <c r="A251" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B251" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" ht="21">
+      <c r="A252" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B252" s="6" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" ht="21">
+      <c r="A253" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B253" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" ht="21">
+      <c r="A254" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B254" s="6" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" ht="21">
+      <c r="A255" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B255" s="6" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" ht="21">
+      <c r="A256" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B256" s="6" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" ht="21">
+      <c r="A257" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B257" s="6" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" ht="21">
+      <c r="A258" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B258" s="6" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" ht="21">
+      <c r="A259" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B259" s="6" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" ht="21">
+      <c r="A260" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B260" s="6" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" ht="21">
+      <c r="A261" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B261" s="6" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" ht="21">
+      <c r="A262" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B262" s="6" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" ht="21">
+      <c r="A263" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B263" s="6" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" ht="21">
+      <c r="A264" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B264" s="6" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" ht="21">
+      <c r="A265" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B265" s="6" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" ht="21">
+      <c r="A266" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B266" s="6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" ht="21">
+      <c r="A267" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B267" s="6" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" ht="21">
+      <c r="A268" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B268" s="6" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" ht="21">
+      <c r="A269" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B269" s="6" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" ht="21">
+      <c r="A270" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B270" s="6" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" ht="21">
+      <c r="A271" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B271" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" ht="21">
+      <c r="A272" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B272" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" ht="21">
+      <c r="B273" s="7"/>
+    </row>
+    <row r="274" spans="1:2" ht="21">
+      <c r="B274" s="7"/>
+    </row>
+    <row r="275" spans="1:2" ht="21">
+      <c r="A275" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B275" s="6" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" ht="21">
+      <c r="A276" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B276" s="6" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" ht="21">
+      <c r="A277" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B277" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" ht="21">
+      <c r="A278" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B278" s="6" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" ht="21">
+      <c r="A279" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B279" s="6" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" ht="21">
+      <c r="A280" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B280" s="6" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" ht="21">
+      <c r="A281" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B281" s="6" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" ht="21">
+      <c r="A282" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B282" s="6" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" ht="21">
+      <c r="A283" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B283" s="6" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" ht="21">
+      <c r="A284" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B284" s="6" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" ht="21">
+      <c r="A285" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B285" s="6" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" ht="21">
+      <c r="A286" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B286" s="6" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" ht="21">
+      <c r="A287" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B287" s="6" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" ht="21">
+      <c r="A288" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B288" s="6" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" ht="21">
+      <c r="A289" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B289" s="6" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" ht="21">
+      <c r="A290" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B290" s="6" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" ht="21">
+      <c r="A291" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B291" s="6" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" ht="21">
+      <c r="A292" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B292" s="6" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" ht="21">
+      <c r="A293" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B293" s="6" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" ht="21">
+      <c r="B294" s="7"/>
+    </row>
+    <row r="295" spans="1:2" ht="21">
+      <c r="B295" s="7"/>
+    </row>
+    <row r="296" spans="1:2" ht="21">
+      <c r="A296" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B296" s="6" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" ht="21">
+      <c r="A297" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B297" s="6" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" ht="21">
+      <c r="A298" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B298" s="6" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" ht="21">
+      <c r="A299" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B299" s="6" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" ht="21">
+      <c r="A300" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B300" s="6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" ht="21">
+      <c r="A301" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B301" s="6" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" ht="21">
+      <c r="A302" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B302" s="6" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" ht="21">
+      <c r="A303" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B303" s="6" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" ht="21">
+      <c r="A304" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B304" s="6" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" ht="21">
+      <c r="A305" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B305" s="6" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" ht="21">
+      <c r="A306" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B306" s="6" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" ht="21">
+      <c r="A307" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B307" s="6" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" ht="21">
+      <c r="A308" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B308" s="6" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" ht="21">
+      <c r="A309" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B309" s="9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" ht="21">
+      <c r="A310" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B310" s="6" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" ht="21">
+      <c r="A311" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B311" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" ht="21">
+      <c r="A312" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B312" s="6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" ht="21">
+      <c r="A313" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B313" s="6" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" ht="21">
+      <c r="A314" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B314" s="6" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" ht="21">
+      <c r="A315" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B315" s="6" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" ht="21">
+      <c r="A316" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B316" s="6" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" ht="21">
+      <c r="A317" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B317" s="6" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" ht="21">
+      <c r="A318" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B318" s="6" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" ht="21">
+      <c r="A319" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B319" s="6" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" ht="21">
+      <c r="A320" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B320" s="6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" ht="21">
+      <c r="A321" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B321" s="6" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" ht="21">
+      <c r="A322" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B322" s="6" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" ht="21">
+      <c r="A323" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B323" s="6" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" ht="21">
+      <c r="A324" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B324" s="6" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" ht="21">
+      <c r="A325" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B325" s="6" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" ht="21">
+      <c r="A326" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B326" s="6" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" ht="21">
+      <c r="A327" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B327" s="6" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" ht="21">
+      <c r="A328" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B328" s="6" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" ht="21">
+      <c r="A329" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B329" s="6" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" ht="21">
+      <c r="A330" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B330" s="6" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" ht="21">
+      <c r="A331" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B331" s="6" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" ht="21">
+      <c r="A332" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B332" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" ht="21">
+      <c r="A333" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B333" s="6" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" ht="21">
+      <c r="B334" s="7"/>
+    </row>
+    <row r="335" spans="1:2" ht="21">
+      <c r="B335" s="7"/>
+    </row>
+    <row r="336" spans="1:2" ht="21">
+      <c r="A336" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="B336" s="6" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" ht="21">
+      <c r="A337" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="B337" s="6" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" ht="21">
+      <c r="A338" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="B338" s="6" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" ht="21">
+      <c r="A339" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="B339" s="6" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" ht="21">
+      <c r="A340" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="B340" s="6" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" ht="21">
+      <c r="A341" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="B341" s="6" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" ht="21">
+      <c r="A342" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="B342" s="6" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" ht="21">
+      <c r="A343" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="B343" s="6" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" ht="21">
+      <c r="A344" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="B344" s="9" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" ht="21">
+      <c r="A345" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="B345" s="6" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" ht="21">
+      <c r="A346" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="B346" s="6" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" ht="21">
+      <c r="A347" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="B347" s="6" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" ht="21">
+      <c r="A348" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="B348" s="6" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" ht="21">
+      <c r="A349" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="B349" s="6" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" ht="21">
+      <c r="A350" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="B350" s="6" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" ht="21">
+      <c r="A351" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="B351" s="6" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" ht="21">
+      <c r="A352" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="B352" s="6" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" ht="21">
+      <c r="A353" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="B353" s="6" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2" ht="21">
+      <c r="B354" s="7"/>
+    </row>
+    <row r="355" spans="1:2" ht="21">
+      <c r="B355" s="7"/>
+    </row>
+    <row r="356" spans="1:2" ht="21">
+      <c r="A356" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B356" s="6" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" ht="21">
+      <c r="A357" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B357" s="6" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" ht="21">
+      <c r="A358" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B358" s="6" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" ht="21">
+      <c r="A359" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B359" s="6" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" ht="21">
+      <c r="A360" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B360" s="6" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" ht="21">
+      <c r="A361" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B361" s="6" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2" ht="21">
+      <c r="A362" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B362" s="6" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2" ht="21">
+      <c r="A363" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B363" s="6" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" ht="21">
+      <c r="A364" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B364" s="6" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2" ht="21">
+      <c r="A365" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B365" s="6" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2" ht="21">
+      <c r="A366" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B366" s="6" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" ht="21">
+      <c r="A367" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B367" s="6" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2" ht="21">
+      <c r="A368" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B368" s="6" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2" ht="21">
+      <c r="A369" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B369" s="6" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2" ht="21">
+      <c r="A370" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B370" s="6" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2" ht="21">
+      <c r="A371" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B371" s="6" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2" ht="21">
+      <c r="A372" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B372" s="6" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2" ht="21">
+      <c r="A373" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B373" s="6" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2" ht="21">
+      <c r="A374" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B374" s="6" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2" ht="21">
+      <c r="A375" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B375" s="6" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2" ht="21">
+      <c r="A376" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B376" s="6" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2" ht="21">
+      <c r="A377" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B377" s="6" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2" ht="21">
+      <c r="A378" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B378" s="6" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="379" spans="1:2" ht="21">
+      <c r="A379" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B379" s="6" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2" ht="21">
+      <c r="A380" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B380" s="6" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="381" spans="1:2" ht="21">
+      <c r="A381" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B381" s="6" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2" ht="21">
+      <c r="A382" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B382" s="6" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2" ht="21">
+      <c r="A383" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B383" s="6" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2" ht="21">
+      <c r="A384" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B384" s="6" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2" ht="21">
+      <c r="A385" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B385" s="6" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2" ht="21">
+      <c r="A386" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B386" s="6" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="387" spans="1:2" ht="21">
+      <c r="A387" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B387" s="6" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2" ht="21">
+      <c r="A388" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B388" s="6" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="389" spans="1:2" ht="21">
+      <c r="A389" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B389" s="6" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="390" spans="1:2" ht="21">
+      <c r="A390" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B390" s="6" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="391" spans="1:2" ht="21">
+      <c r="A391" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B391" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="392" spans="1:2" ht="21">
+      <c r="A392" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B392" s="6" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="393" spans="1:2" ht="21">
+      <c r="A393" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B393" s="6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="394" spans="1:2" ht="21">
+      <c r="A394" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B394" s="6" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="395" spans="1:2" ht="21">
+      <c r="A395" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B395" s="6" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="396" spans="1:2" ht="21">
+      <c r="A396" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B396" s="6" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="397" spans="1:2" ht="21">
+      <c r="A397" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B397" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="398" spans="1:2" ht="21">
+      <c r="A398" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B398" s="6" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="399" spans="1:2" ht="21">
+      <c r="A399" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B399" s="6" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="400" spans="1:2" ht="21">
+      <c r="B400" s="7"/>
+    </row>
+    <row r="401" spans="1:2" ht="21">
+      <c r="B401" s="7"/>
+    </row>
+    <row r="402" spans="1:2" ht="21">
+      <c r="A402" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="B402" s="6" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="403" spans="1:2" ht="21">
+      <c r="A403" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="B403" s="6" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="404" spans="1:2" ht="21">
+      <c r="A404" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="B404" s="6" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="405" spans="1:2" ht="21">
+      <c r="A405" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="B405" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="406" spans="1:2" ht="21">
+      <c r="A406" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="B406" s="6" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="407" spans="1:2" ht="21">
+      <c r="A407" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="B407" s="6" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="408" spans="1:2" ht="21">
+      <c r="B408" s="7"/>
+    </row>
+    <row r="409" spans="1:2" ht="21">
+      <c r="B409" s="7"/>
+    </row>
+    <row r="410" spans="1:2" ht="21">
+      <c r="A410" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B410" s="6" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="411" spans="1:2" ht="21">
+      <c r="A411" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B411" s="6" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="412" spans="1:2" ht="21">
+      <c r="A412" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B412" s="6" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="413" spans="1:2" ht="21">
+      <c r="A413" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B413" s="6" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="414" spans="1:2" ht="21">
+      <c r="A414" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B414" s="6" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="415" spans="1:2" ht="21">
+      <c r="A415" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B415" s="6" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="416" spans="1:2" ht="21">
+      <c r="A416" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B416" s="6" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="417" spans="1:2" ht="21">
+      <c r="A417" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B417" s="6" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="418" spans="1:2" ht="21">
+      <c r="A418" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B418" s="6" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="419" spans="1:2" ht="21">
+      <c r="A419" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B419" s="6" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="420" spans="1:2" ht="21">
+      <c r="A420" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B420" s="6" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="421" spans="1:2" ht="21">
+      <c r="A421" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B421" s="6" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="422" spans="1:2" ht="21">
+      <c r="A422" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B422" s="6" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="423" spans="1:2" ht="21">
+      <c r="A423" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B423" s="6" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="424" spans="1:2" ht="21">
+      <c r="A424" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B424" s="6" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="425" spans="1:2" ht="21">
+      <c r="A425" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B425" s="6" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="426" spans="1:2" ht="21">
+      <c r="A426" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B426" s="6" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="427" spans="1:2" ht="21">
+      <c r="A427" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B427" s="6" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="428" spans="1:2" ht="21">
+      <c r="A428" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B428" s="6" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="429" spans="1:2" ht="21">
+      <c r="A429" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B429" s="6" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="430" spans="1:2" ht="21">
+      <c r="A430" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B430" s="6" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="431" spans="1:2" ht="21">
+      <c r="A431" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B431" s="6" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="432" spans="1:2" ht="21">
+      <c r="A432" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B432" s="6" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="433" spans="1:2" ht="21">
+      <c r="A433" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B433" s="6" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="434" spans="1:2" ht="21">
+      <c r="A434" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B434" s="6" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="435" spans="1:2" ht="21">
+      <c r="A435" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B435" s="6" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="436" spans="1:2" ht="21">
+      <c r="A436" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B436" s="6" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="437" spans="1:2" ht="21">
+      <c r="A437" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B437" s="6" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="438" spans="1:2" ht="21">
+      <c r="A438" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B438" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="439" spans="1:2" ht="21">
+      <c r="A439" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B439" s="6" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="440" spans="1:2" ht="21">
+      <c r="A440" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B440" s="6" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="441" spans="1:2" ht="21">
+      <c r="A441" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B441" s="6" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="442" spans="1:2" ht="21">
+      <c r="A442" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B442" s="6" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="443" spans="1:2" ht="21">
+      <c r="A443" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B443" s="6" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="444" spans="1:2" ht="21">
+      <c r="A444" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B444" s="6" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="445" spans="1:2" ht="21">
+      <c r="A445" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B445" s="6" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="446" spans="1:2" ht="21">
+      <c r="A446" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B446" s="6" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="447" spans="1:2" ht="21">
+      <c r="A447" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B447" s="6" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="448" spans="1:2" ht="21">
+      <c r="A448" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B448" s="6" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="449" spans="1:2" ht="21">
+      <c r="A449" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B449" s="6" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="450" spans="1:2" ht="21">
+      <c r="A450" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B450" s="6" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="451" spans="1:2" ht="21">
+      <c r="A451" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B451" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="452" spans="1:2" ht="21">
+      <c r="A452" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B452" s="6" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="453" spans="1:2" ht="21">
+      <c r="A453" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B453" s="6" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="454" spans="1:2" ht="21">
+      <c r="A454" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B454" s="6" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="455" spans="1:2" ht="21">
+      <c r="A455" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B455" s="6" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="456" spans="1:2" ht="21">
+      <c r="A456" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B456" s="6" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="457" spans="1:2" ht="21">
+      <c r="A457" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B457" s="6" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="458" spans="1:2" ht="21">
+      <c r="A458" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B458" s="6" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="459" spans="1:2" ht="21">
+      <c r="A459" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B459" s="6" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="460" spans="1:2" ht="21">
+      <c r="A460" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B460" s="6" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="461" spans="1:2" ht="21">
+      <c r="A461" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B461" s="6" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="462" spans="1:2" ht="21">
+      <c r="A462" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B462" s="6" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="463" spans="1:2" ht="21">
+      <c r="A463" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B463" s="6" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="464" spans="1:2" ht="21">
+      <c r="A464" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B464" s="6" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="465" spans="1:2" ht="21">
+      <c r="A465" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B465" s="6" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="466" spans="1:2" ht="21">
+      <c r="A466" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B466" s="6" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="467" spans="1:2" ht="21">
+      <c r="A467" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B467" s="6" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="468" spans="1:2" ht="21">
+      <c r="A468" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B468" s="6" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="469" spans="1:2" ht="21">
+      <c r="A469" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B469" s="6" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="470" spans="1:2" ht="21">
+      <c r="B470" s="7"/>
+    </row>
+    <row r="471" spans="1:2" ht="21">
+      <c r="A471" s="8"/>
+      <c r="B471" s="7"/>
+    </row>
+    <row r="472" spans="1:2" ht="21">
+      <c r="A472" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="B472" s="6" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="473" spans="1:2" ht="21">
+      <c r="A473" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="B473" s="6" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="474" spans="1:2" ht="21">
+      <c r="A474" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="B474" s="6" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="475" spans="1:2" ht="21">
+      <c r="A475" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="B475" s="6" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="476" spans="1:2" ht="21">
+      <c r="A476" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="B476" s="6" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="477" spans="1:2" ht="21">
+      <c r="A477" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="B477" s="6" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="478" spans="1:2" ht="21">
+      <c r="A478" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="B478" s="6" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="479" spans="1:2" ht="21">
+      <c r="A479" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="B479" s="6" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="480" spans="1:2" ht="21">
+      <c r="A480" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="B480" s="6" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="481" spans="1:2" ht="21">
+      <c r="A481" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="B481" s="6" t="s">
+        <v>463</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B7" r:id="rId2"/>
+    <hyperlink ref="B8" r:id="rId3"/>
+    <hyperlink ref="B9" r:id="rId4"/>
+    <hyperlink ref="B10" r:id="rId5"/>
+    <hyperlink ref="B11" r:id="rId6"/>
+    <hyperlink ref="B12" r:id="rId7"/>
+    <hyperlink ref="B13" r:id="rId8"/>
+    <hyperlink ref="B14" r:id="rId9"/>
+    <hyperlink ref="B15" r:id="rId10"/>
+    <hyperlink ref="B16" r:id="rId11"/>
+    <hyperlink ref="B17" r:id="rId12"/>
+    <hyperlink ref="B18" r:id="rId13"/>
+    <hyperlink ref="B19" r:id="rId14"/>
+    <hyperlink ref="B20" r:id="rId15"/>
+    <hyperlink ref="B21" r:id="rId16"/>
+    <hyperlink ref="B22" r:id="rId17"/>
+    <hyperlink ref="B23" r:id="rId18"/>
+    <hyperlink ref="B24" r:id="rId19"/>
+    <hyperlink ref="B25" r:id="rId20"/>
+    <hyperlink ref="B26" r:id="rId21"/>
+    <hyperlink ref="B27" r:id="rId22"/>
+    <hyperlink ref="B28" r:id="rId23"/>
+    <hyperlink ref="B29" r:id="rId24"/>
+    <hyperlink ref="B30" r:id="rId25"/>
+    <hyperlink ref="B31" r:id="rId26"/>
+    <hyperlink ref="B32" r:id="rId27"/>
+    <hyperlink ref="B33" r:id="rId28"/>
+    <hyperlink ref="B34" r:id="rId29"/>
+    <hyperlink ref="B35" r:id="rId30"/>
+    <hyperlink ref="B36" r:id="rId31"/>
+    <hyperlink ref="B37" r:id="rId32"/>
+    <hyperlink ref="B38" r:id="rId33"/>
+    <hyperlink ref="B39" r:id="rId34"/>
+    <hyperlink ref="B40" r:id="rId35"/>
+    <hyperlink ref="B41" r:id="rId36"/>
+    <hyperlink ref="B44" r:id="rId37"/>
+    <hyperlink ref="B45" r:id="rId38"/>
+    <hyperlink ref="B46" r:id="rId39"/>
+    <hyperlink ref="B47" r:id="rId40"/>
+    <hyperlink ref="B48" r:id="rId41"/>
+    <hyperlink ref="B49" r:id="rId42"/>
+    <hyperlink ref="B50" r:id="rId43"/>
+    <hyperlink ref="B51" r:id="rId44"/>
+    <hyperlink ref="B52" r:id="rId45"/>
+    <hyperlink ref="B53" r:id="rId46"/>
+    <hyperlink ref="B56" r:id="rId47"/>
+    <hyperlink ref="B57" r:id="rId48"/>
+    <hyperlink ref="B58" r:id="rId49"/>
+    <hyperlink ref="B60" r:id="rId50"/>
+    <hyperlink ref="B61" r:id="rId51"/>
+    <hyperlink ref="B62" r:id="rId52"/>
+    <hyperlink ref="B63" r:id="rId53"/>
+    <hyperlink ref="B64" r:id="rId54"/>
+    <hyperlink ref="B65" r:id="rId55"/>
+    <hyperlink ref="B66" r:id="rId56"/>
+    <hyperlink ref="B67" r:id="rId57"/>
+    <hyperlink ref="B68" r:id="rId58"/>
+    <hyperlink ref="B69" r:id="rId59"/>
+    <hyperlink ref="B70" r:id="rId60"/>
+    <hyperlink ref="B71" r:id="rId61"/>
+    <hyperlink ref="B72" r:id="rId62"/>
+    <hyperlink ref="B73" r:id="rId63"/>
+    <hyperlink ref="B74" r:id="rId64"/>
+    <hyperlink ref="B75" r:id="rId65"/>
+    <hyperlink ref="B76" r:id="rId66"/>
+    <hyperlink ref="B77" r:id="rId67"/>
+    <hyperlink ref="B78" r:id="rId68"/>
+    <hyperlink ref="B79" r:id="rId69"/>
+    <hyperlink ref="B80" r:id="rId70"/>
+    <hyperlink ref="B81" r:id="rId71"/>
+    <hyperlink ref="B82" r:id="rId72"/>
+    <hyperlink ref="B83" r:id="rId73"/>
+    <hyperlink ref="B84" r:id="rId74"/>
+    <hyperlink ref="B85" r:id="rId75"/>
+    <hyperlink ref="B86" r:id="rId76"/>
+    <hyperlink ref="B87" r:id="rId77"/>
+    <hyperlink ref="B88" r:id="rId78"/>
+    <hyperlink ref="B89" r:id="rId79"/>
+    <hyperlink ref="B90" r:id="rId80"/>
+    <hyperlink ref="B91" r:id="rId81"/>
+    <hyperlink ref="B92" r:id="rId82"/>
+    <hyperlink ref="B93" r:id="rId83"/>
+    <hyperlink ref="B94" r:id="rId84"/>
+    <hyperlink ref="B95" r:id="rId85"/>
+    <hyperlink ref="B96" r:id="rId86"/>
+    <hyperlink ref="B97" r:id="rId87"/>
+    <hyperlink ref="B98" r:id="rId88"/>
+    <hyperlink ref="B101" r:id="rId89"/>
+    <hyperlink ref="B102" r:id="rId90"/>
+    <hyperlink ref="B103" r:id="rId91"/>
+    <hyperlink ref="B104" r:id="rId92"/>
+    <hyperlink ref="B106" r:id="rId93" location=":~:text=We%20need%20to%20find%20a,set%20of%20points%20is%20minimum.&amp;text=In%20above%20figure%20optimum%20location,is%20minimum%20obtainable%20total%20distance."/>
+    <hyperlink ref="B107" r:id="rId94"/>
+    <hyperlink ref="B108" r:id="rId95"/>
+    <hyperlink ref="B109" r:id="rId96"/>
+    <hyperlink ref="B110" r:id="rId97"/>
+    <hyperlink ref="B111" r:id="rId98"/>
+    <hyperlink ref="B113" r:id="rId99"/>
+    <hyperlink ref="B114" r:id="rId100"/>
+    <hyperlink ref="B115" r:id="rId101"/>
+    <hyperlink ref="B116" r:id="rId102"/>
+    <hyperlink ref="B117" r:id="rId103"/>
+    <hyperlink ref="B118" r:id="rId104"/>
+    <hyperlink ref="B119" r:id="rId105"/>
+    <hyperlink ref="B120" r:id="rId106"/>
+    <hyperlink ref="B121" r:id="rId107"/>
+    <hyperlink ref="B122" r:id="rId108"/>
+    <hyperlink ref="B123" r:id="rId109"/>
+    <hyperlink ref="B124" r:id="rId110"/>
+    <hyperlink ref="B125" r:id="rId111"/>
+    <hyperlink ref="B126" r:id="rId112"/>
+    <hyperlink ref="B127" r:id="rId113"/>
+    <hyperlink ref="B128" r:id="rId114"/>
+    <hyperlink ref="B129" r:id="rId115"/>
+    <hyperlink ref="B130" r:id="rId116"/>
+    <hyperlink ref="B131" r:id="rId117"/>
+    <hyperlink ref="B132" r:id="rId118"/>
+    <hyperlink ref="B133" r:id="rId119"/>
+    <hyperlink ref="B134" r:id="rId120"/>
+    <hyperlink ref="B135" r:id="rId121"/>
+    <hyperlink ref="B136" r:id="rId122"/>
+    <hyperlink ref="B105" r:id="rId123"/>
+    <hyperlink ref="B112" r:id="rId124"/>
+    <hyperlink ref="B139" r:id="rId125"/>
+    <hyperlink ref="B140" r:id="rId126"/>
+    <hyperlink ref="B141" r:id="rId127"/>
+    <hyperlink ref="B142" r:id="rId128"/>
+    <hyperlink ref="B143" r:id="rId129"/>
+    <hyperlink ref="B144" r:id="rId130"/>
+    <hyperlink ref="B145" r:id="rId131"/>
+    <hyperlink ref="B146" r:id="rId132"/>
+    <hyperlink ref="B147" r:id="rId133"/>
+    <hyperlink ref="B148" r:id="rId134"/>
+    <hyperlink ref="B149" r:id="rId135"/>
+    <hyperlink ref="B150" r:id="rId136"/>
+    <hyperlink ref="B151" r:id="rId137"/>
+    <hyperlink ref="B152" r:id="rId138"/>
+    <hyperlink ref="B153" r:id="rId139"/>
+    <hyperlink ref="B154" r:id="rId140"/>
+    <hyperlink ref="B155" r:id="rId141"/>
+    <hyperlink ref="B156" r:id="rId142"/>
+    <hyperlink ref="B157" r:id="rId143"/>
+    <hyperlink ref="B158" r:id="rId144"/>
+    <hyperlink ref="B159" r:id="rId145"/>
+    <hyperlink ref="B160" r:id="rId146"/>
+    <hyperlink ref="B161" r:id="rId147"/>
+    <hyperlink ref="B162" r:id="rId148"/>
+    <hyperlink ref="B163" r:id="rId149"/>
+    <hyperlink ref="B166" r:id="rId150"/>
+    <hyperlink ref="B167" r:id="rId151"/>
+    <hyperlink ref="B168" r:id="rId152"/>
+    <hyperlink ref="B169" r:id="rId153"/>
+    <hyperlink ref="B170" r:id="rId154"/>
+    <hyperlink ref="B171" r:id="rId155"/>
+    <hyperlink ref="B172" r:id="rId156"/>
+    <hyperlink ref="B173" r:id="rId157"/>
+    <hyperlink ref="B174" r:id="rId158"/>
+    <hyperlink ref="B177" r:id="rId159"/>
+    <hyperlink ref="B178" r:id="rId160"/>
+    <hyperlink ref="B179" r:id="rId161"/>
+    <hyperlink ref="B180" r:id="rId162"/>
+    <hyperlink ref="B181" r:id="rId163"/>
+    <hyperlink ref="B182" r:id="rId164"/>
+    <hyperlink ref="B183" r:id="rId165"/>
+    <hyperlink ref="B184" r:id="rId166"/>
+    <hyperlink ref="B185" r:id="rId167"/>
+    <hyperlink ref="B186" r:id="rId168"/>
+    <hyperlink ref="B187" r:id="rId169"/>
+    <hyperlink ref="B188" r:id="rId170"/>
+    <hyperlink ref="B189" r:id="rId171"/>
+    <hyperlink ref="B190" r:id="rId172"/>
+    <hyperlink ref="B191" r:id="rId173"/>
+    <hyperlink ref="B192" r:id="rId174"/>
+    <hyperlink ref="B193" r:id="rId175"/>
+    <hyperlink ref="B194" r:id="rId176"/>
+    <hyperlink ref="B195" r:id="rId177"/>
+    <hyperlink ref="B196" r:id="rId178"/>
+    <hyperlink ref="B197" r:id="rId179" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010."/>
+    <hyperlink ref="B198" r:id="rId180"/>
+    <hyperlink ref="B199" r:id="rId181"/>
+    <hyperlink ref="B200" r:id="rId182"/>
+    <hyperlink ref="B201" r:id="rId183"/>
+    <hyperlink ref="B202" r:id="rId184"/>
+    <hyperlink ref="B203" r:id="rId185" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not."/>
+    <hyperlink ref="B204" r:id="rId186"/>
+    <hyperlink ref="B205" r:id="rId187"/>
+    <hyperlink ref="B206" r:id="rId188"/>
+    <hyperlink ref="B207" r:id="rId189"/>
+    <hyperlink ref="B208" r:id="rId190"/>
+    <hyperlink ref="B209" r:id="rId191"/>
+    <hyperlink ref="B210" r:id="rId192"/>
+    <hyperlink ref="B211" r:id="rId193"/>
+    <hyperlink ref="B214" r:id="rId194"/>
+    <hyperlink ref="B215" r:id="rId195"/>
+    <hyperlink ref="B216" r:id="rId196"/>
+    <hyperlink ref="B217" r:id="rId197"/>
+    <hyperlink ref="B218" r:id="rId198"/>
+    <hyperlink ref="B219" r:id="rId199"/>
+    <hyperlink ref="B220" r:id="rId200"/>
+    <hyperlink ref="B221" r:id="rId201"/>
+    <hyperlink ref="B222" r:id="rId202"/>
+    <hyperlink ref="B223" r:id="rId203"/>
+    <hyperlink ref="B224" r:id="rId204"/>
+    <hyperlink ref="B225" r:id="rId205"/>
+    <hyperlink ref="B226" r:id="rId206"/>
+    <hyperlink ref="B227" r:id="rId207"/>
+    <hyperlink ref="B228" r:id="rId208"/>
+    <hyperlink ref="B229" r:id="rId209"/>
+    <hyperlink ref="B230" r:id="rId210"/>
+    <hyperlink ref="B231" r:id="rId211"/>
+    <hyperlink ref="B232" r:id="rId212"/>
+    <hyperlink ref="B233" r:id="rId213"/>
+    <hyperlink ref="B234" r:id="rId214"/>
+    <hyperlink ref="B235" r:id="rId215"/>
+    <hyperlink ref="B238" r:id="rId216"/>
+    <hyperlink ref="B239" r:id="rId217"/>
+    <hyperlink ref="B240" r:id="rId218"/>
+    <hyperlink ref="B241" r:id="rId219"/>
+    <hyperlink ref="B242" r:id="rId220"/>
+    <hyperlink ref="B243" r:id="rId221"/>
+    <hyperlink ref="B244" r:id="rId222"/>
+    <hyperlink ref="B245" r:id="rId223"/>
+    <hyperlink ref="B246" r:id="rId224"/>
+    <hyperlink ref="B247" r:id="rId225"/>
+    <hyperlink ref="B248" r:id="rId226"/>
+    <hyperlink ref="B249" r:id="rId227"/>
+    <hyperlink ref="B250" r:id="rId228"/>
+    <hyperlink ref="B251" r:id="rId229"/>
+    <hyperlink ref="B252" r:id="rId230"/>
+    <hyperlink ref="B253" r:id="rId231"/>
+    <hyperlink ref="B254" r:id="rId232"/>
+    <hyperlink ref="B255" r:id="rId233"/>
+    <hyperlink ref="B256" r:id="rId234"/>
+    <hyperlink ref="B257" r:id="rId235" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S."/>
+    <hyperlink ref="B258" r:id="rId236"/>
+    <hyperlink ref="B259" r:id="rId237"/>
+    <hyperlink ref="B260" r:id="rId238"/>
+    <hyperlink ref="B261" r:id="rId239"/>
+    <hyperlink ref="B262" r:id="rId240"/>
+    <hyperlink ref="B263" r:id="rId241"/>
+    <hyperlink ref="B264" r:id="rId242"/>
+    <hyperlink ref="B265" r:id="rId243"/>
+    <hyperlink ref="B266" r:id="rId244"/>
+    <hyperlink ref="B267" r:id="rId245"/>
+    <hyperlink ref="B268" r:id="rId246"/>
+    <hyperlink ref="B269" r:id="rId247"/>
+    <hyperlink ref="B270" r:id="rId248"/>
+    <hyperlink ref="B271" r:id="rId249"/>
+    <hyperlink ref="B272" r:id="rId250"/>
+    <hyperlink ref="B275" r:id="rId251"/>
+    <hyperlink ref="B276" r:id="rId252"/>
+    <hyperlink ref="B277" r:id="rId253"/>
+    <hyperlink ref="B278" r:id="rId254"/>
+    <hyperlink ref="B279" r:id="rId255"/>
+    <hyperlink ref="B280" r:id="rId256"/>
+    <hyperlink ref="B281" r:id="rId257"/>
+    <hyperlink ref="B282" r:id="rId258"/>
+    <hyperlink ref="B283" r:id="rId259"/>
+    <hyperlink ref="B284" r:id="rId260"/>
+    <hyperlink ref="B285" r:id="rId261"/>
+    <hyperlink ref="B286" r:id="rId262"/>
+    <hyperlink ref="B287" r:id="rId263"/>
+    <hyperlink ref="B288" r:id="rId264"/>
+    <hyperlink ref="B289" r:id="rId265"/>
+    <hyperlink ref="B290" r:id="rId266"/>
+    <hyperlink ref="B291" r:id="rId267"/>
+    <hyperlink ref="B292" r:id="rId268"/>
+    <hyperlink ref="B293" r:id="rId269"/>
+    <hyperlink ref="B296" r:id="rId270"/>
+    <hyperlink ref="B297" r:id="rId271"/>
+    <hyperlink ref="B298" r:id="rId272"/>
+    <hyperlink ref="B299" r:id="rId273"/>
+    <hyperlink ref="B300" r:id="rId274"/>
+    <hyperlink ref="B301" r:id="rId275"/>
+    <hyperlink ref="B302" r:id="rId276"/>
+    <hyperlink ref="B303" r:id="rId277"/>
+    <hyperlink ref="B304" r:id="rId278"/>
+    <hyperlink ref="B305" r:id="rId279"/>
+    <hyperlink ref="B306" r:id="rId280" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)."/>
+    <hyperlink ref="B307" r:id="rId281"/>
+    <hyperlink ref="B308" r:id="rId282"/>
+    <hyperlink ref="B309" r:id="rId283"/>
+    <hyperlink ref="B310" r:id="rId284"/>
+    <hyperlink ref="B311" r:id="rId285"/>
+    <hyperlink ref="B312" r:id="rId286"/>
+    <hyperlink ref="B313" r:id="rId287"/>
+    <hyperlink ref="B314" r:id="rId288"/>
+    <hyperlink ref="B315" r:id="rId289"/>
+    <hyperlink ref="B316" r:id="rId290"/>
+    <hyperlink ref="B317" r:id="rId291"/>
+    <hyperlink ref="B318" r:id="rId292"/>
+    <hyperlink ref="B319" r:id="rId293"/>
+    <hyperlink ref="B320" r:id="rId294"/>
+    <hyperlink ref="B321" r:id="rId295"/>
+    <hyperlink ref="B322" r:id="rId296"/>
+    <hyperlink ref="B323" r:id="rId297"/>
+    <hyperlink ref="B324" r:id="rId298"/>
+    <hyperlink ref="B325" r:id="rId299"/>
+    <hyperlink ref="B326" r:id="rId300"/>
+    <hyperlink ref="B327" r:id="rId301"/>
+    <hyperlink ref="B328" r:id="rId302"/>
+    <hyperlink ref="B329" r:id="rId303"/>
+    <hyperlink ref="B330" r:id="rId304"/>
+    <hyperlink ref="B331" r:id="rId305"/>
+    <hyperlink ref="B332" r:id="rId306"/>
+    <hyperlink ref="B333" r:id="rId307"/>
+    <hyperlink ref="B336" r:id="rId308"/>
+    <hyperlink ref="B337" r:id="rId309"/>
+    <hyperlink ref="B338" r:id="rId310"/>
+    <hyperlink ref="B339" r:id="rId311"/>
+    <hyperlink ref="B340" r:id="rId312"/>
+    <hyperlink ref="B341" r:id="rId313"/>
+    <hyperlink ref="B342" r:id="rId314"/>
+    <hyperlink ref="B343" r:id="rId315"/>
+    <hyperlink ref="B344" r:id="rId316"/>
+    <hyperlink ref="B345" r:id="rId317"/>
+    <hyperlink ref="B346" r:id="rId318"/>
+    <hyperlink ref="B347" r:id="rId319"/>
+    <hyperlink ref="B348" r:id="rId320"/>
+    <hyperlink ref="B349" r:id="rId321"/>
+    <hyperlink ref="B350" r:id="rId322"/>
+    <hyperlink ref="B351" r:id="rId323"/>
+    <hyperlink ref="B352" r:id="rId324"/>
+    <hyperlink ref="B353" r:id="rId325"/>
+    <hyperlink ref="B357" r:id="rId326"/>
+    <hyperlink ref="B358" r:id="rId327"/>
+    <hyperlink ref="B359" r:id="rId328"/>
+    <hyperlink ref="B360" r:id="rId329"/>
+    <hyperlink ref="B361" r:id="rId330"/>
+    <hyperlink ref="B362" r:id="rId331"/>
+    <hyperlink ref="B363" r:id="rId332"/>
+    <hyperlink ref="B364" r:id="rId333"/>
+    <hyperlink ref="B365" r:id="rId334"/>
+    <hyperlink ref="B366" r:id="rId335"/>
+    <hyperlink ref="B367" r:id="rId336"/>
+    <hyperlink ref="B368" r:id="rId337"/>
+    <hyperlink ref="B369" r:id="rId338"/>
+    <hyperlink ref="B370" r:id="rId339"/>
+    <hyperlink ref="B371" r:id="rId340"/>
+    <hyperlink ref="B372" r:id="rId341"/>
+    <hyperlink ref="B373" r:id="rId342"/>
+    <hyperlink ref="B374" r:id="rId343"/>
+    <hyperlink ref="B375" r:id="rId344"/>
+    <hyperlink ref="B376" r:id="rId345"/>
+    <hyperlink ref="B377" r:id="rId346"/>
+    <hyperlink ref="B378" r:id="rId347"/>
+    <hyperlink ref="B379" r:id="rId348" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color."/>
+    <hyperlink ref="B380" r:id="rId349"/>
+    <hyperlink ref="B381" r:id="rId350"/>
+    <hyperlink ref="B382" r:id="rId351"/>
+    <hyperlink ref="B383" r:id="rId352"/>
+    <hyperlink ref="B384" r:id="rId353"/>
+    <hyperlink ref="B385" r:id="rId354"/>
+    <hyperlink ref="B386" r:id="rId355"/>
+    <hyperlink ref="B387" r:id="rId356"/>
+    <hyperlink ref="B388" r:id="rId357"/>
+    <hyperlink ref="B389" r:id="rId358"/>
+    <hyperlink ref="B390" r:id="rId359"/>
+    <hyperlink ref="B391" r:id="rId360"/>
+    <hyperlink ref="B392" r:id="rId361"/>
+    <hyperlink ref="B393" r:id="rId362"/>
+    <hyperlink ref="B394" r:id="rId363"/>
+    <hyperlink ref="B396" r:id="rId364"/>
+    <hyperlink ref="B395" r:id="rId365"/>
+    <hyperlink ref="B397" r:id="rId366"/>
+    <hyperlink ref="B398" r:id="rId367"/>
+    <hyperlink ref="B399" r:id="rId368"/>
+    <hyperlink ref="B402" r:id="rId369"/>
+    <hyperlink ref="B403" r:id="rId370"/>
+    <hyperlink ref="B404" r:id="rId371"/>
+    <hyperlink ref="B405" r:id="rId372"/>
+    <hyperlink ref="B406" r:id="rId373"/>
+    <hyperlink ref="B407" r:id="rId374"/>
+    <hyperlink ref="B410" r:id="rId375"/>
+    <hyperlink ref="B411" r:id="rId376"/>
+    <hyperlink ref="B412" r:id="rId377"/>
+    <hyperlink ref="B413" r:id="rId378"/>
+    <hyperlink ref="B414" r:id="rId379"/>
+    <hyperlink ref="B415" r:id="rId380"/>
+    <hyperlink ref="B416" r:id="rId381"/>
+    <hyperlink ref="B417" r:id="rId382"/>
+    <hyperlink ref="B418" r:id="rId383"/>
+    <hyperlink ref="B419" r:id="rId384"/>
+    <hyperlink ref="B420" r:id="rId385"/>
+    <hyperlink ref="B421" r:id="rId386"/>
+    <hyperlink ref="B422" r:id="rId387"/>
+    <hyperlink ref="B423" r:id="rId388"/>
+    <hyperlink ref="B424" r:id="rId389"/>
+    <hyperlink ref="B425" r:id="rId390"/>
+    <hyperlink ref="B426" r:id="rId391"/>
+    <hyperlink ref="B427" r:id="rId392"/>
+    <hyperlink ref="B428" r:id="rId393"/>
+    <hyperlink ref="B429" r:id="rId394"/>
+    <hyperlink ref="B430" r:id="rId395"/>
+    <hyperlink ref="B431" r:id="rId396"/>
+    <hyperlink ref="B432" r:id="rId397"/>
+    <hyperlink ref="B433" r:id="rId398"/>
+    <hyperlink ref="B434" r:id="rId399"/>
+    <hyperlink ref="B435" r:id="rId400"/>
+    <hyperlink ref="B436" r:id="rId401"/>
+    <hyperlink ref="B437" r:id="rId402"/>
+    <hyperlink ref="B438" r:id="rId403"/>
+    <hyperlink ref="B439" r:id="rId404"/>
+    <hyperlink ref="B440" r:id="rId405"/>
+    <hyperlink ref="B441" r:id="rId406"/>
+    <hyperlink ref="B442" r:id="rId407"/>
+    <hyperlink ref="B443" r:id="rId408"/>
+    <hyperlink ref="B444" r:id="rId409"/>
+    <hyperlink ref="B445" r:id="rId410"/>
+    <hyperlink ref="B446" r:id="rId411"/>
+    <hyperlink ref="B447" r:id="rId412"/>
+    <hyperlink ref="B448" r:id="rId413"/>
+    <hyperlink ref="B449" r:id="rId414"/>
+    <hyperlink ref="B451" r:id="rId415"/>
+    <hyperlink ref="B450" r:id="rId416"/>
+    <hyperlink ref="B452" r:id="rId417"/>
+    <hyperlink ref="B453" r:id="rId418"/>
+    <hyperlink ref="B454" r:id="rId419"/>
+    <hyperlink ref="B455" r:id="rId420"/>
+    <hyperlink ref="B456" r:id="rId421"/>
+    <hyperlink ref="B457" r:id="rId422"/>
+    <hyperlink ref="B458" r:id="rId423"/>
+    <hyperlink ref="B459" r:id="rId424"/>
+    <hyperlink ref="B460" r:id="rId425"/>
+    <hyperlink ref="B461" r:id="rId426"/>
+    <hyperlink ref="B462" r:id="rId427"/>
+    <hyperlink ref="B469" r:id="rId428"/>
+    <hyperlink ref="B468" r:id="rId429"/>
+    <hyperlink ref="B467" r:id="rId430"/>
+    <hyperlink ref="B466" r:id="rId431"/>
+    <hyperlink ref="B465" r:id="rId432"/>
+    <hyperlink ref="B464" r:id="rId433"/>
+    <hyperlink ref="B463" r:id="rId434"/>
+    <hyperlink ref="B472" r:id="rId435"/>
+    <hyperlink ref="B473" r:id="rId436"/>
+    <hyperlink ref="B474" r:id="rId437"/>
+    <hyperlink ref="B475" r:id="rId438"/>
+    <hyperlink ref="B476" r:id="rId439"/>
+    <hyperlink ref="B477" r:id="rId440"/>
+    <hyperlink ref="B478" r:id="rId441"/>
+    <hyperlink ref="B481" r:id="rId442"/>
+    <hyperlink ref="B479" r:id="rId443"/>
+    <hyperlink ref="B480" r:id="rId444" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result."/>
+    <hyperlink ref="B356" r:id="rId445"/>
+    <hyperlink ref="B2" r:id="rId446"/>
+    <hyperlink ref="C7" r:id="rId447"/>
+    <hyperlink ref="C6" r:id="rId448"/>
+    <hyperlink ref="C8" r:id="rId449"/>
+    <hyperlink ref="C9" r:id="rId450"/>
+    <hyperlink ref="C10" r:id="rId451"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>